<commit_message>
Push choices sheet display.text into display.title.text  Also push display.image into display.title.image
</commit_message>
<xml_diff>
--- a/app/config/assets/framework/forms/framework.opendatakit-2/framework.opendatakit-2.xlsx
+++ b/app/config/assets/framework/forms/framework.opendatakit-2/framework.opendatakit-2.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="4215" yWindow="1335" windowWidth="24297" windowHeight="17097" firstSheet="1" activeTab="2"/>
+    <workbookView xWindow="4215" yWindow="1335" windowWidth="24297" windowHeight="17097" firstSheet="1" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="initial" sheetId="5" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="165">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="164">
   <si>
     <t>comments</t>
   </si>
@@ -46,9 +46,6 @@
   </si>
   <si>
     <t>form_version</t>
-  </si>
-  <si>
-    <t>display.text</t>
   </si>
   <si>
     <t>setting_name</t>
@@ -1110,12 +1107,12 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>
@@ -1149,54 +1146,54 @@
   <sheetData>
     <row r="1" spans="1:9" ht="17.55" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E1" t="s">
         <v>1</v>
       </c>
       <c r="F1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G1" t="s">
+        <v>161</v>
+      </c>
+      <c r="H1" t="s">
         <v>162</v>
-      </c>
-      <c r="H1" t="s">
-        <v>163</v>
       </c>
       <c r="I1" s="2"/>
     </row>
     <row r="2" spans="1:9" ht="17.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D2" t="s">
         <v>17</v>
-      </c>
-      <c r="D2" t="s">
-        <v>18</v>
       </c>
       <c r="I2" s="2"/>
     </row>
     <row r="3" spans="1:9" ht="17.55" customHeight="1" x14ac:dyDescent="0.2">
       <c r="E3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="17.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="I4" s="2"/>
     </row>
@@ -1205,116 +1202,116 @@
         <v>2</v>
       </c>
       <c r="G5" t="s">
+        <v>10</v>
+      </c>
+      <c r="H5" t="s">
         <v>11</v>
-      </c>
-      <c r="H5" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="17.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="17.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="17.55" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="65.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="3"/>
       <c r="B9" s="4" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="E9" t="s">
+        <v>29</v>
+      </c>
+      <c r="G9" t="s">
         <v>30</v>
-      </c>
-      <c r="G9" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="10" spans="1:9" ht="17.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="3"/>
       <c r="B10" s="3"/>
       <c r="C10" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="11" spans="1:9" ht="17.55" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="12" spans="1:9" ht="65.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="3"/>
       <c r="B12" s="4" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="E12" t="s">
+        <v>29</v>
+      </c>
+      <c r="G12" t="s">
         <v>30</v>
-      </c>
-      <c r="G12" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="13" spans="1:9" ht="17.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="3"/>
       <c r="B13" s="3"/>
       <c r="C13" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="14" spans="1:9" ht="17.55" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="15" spans="1:9" ht="65.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="3"/>
       <c r="B15" s="4" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="E15" t="s">
+        <v>29</v>
+      </c>
+      <c r="G15" t="s">
         <v>30</v>
-      </c>
-      <c r="G15" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="16" spans="1:9" ht="17.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="3"/>
       <c r="B16" s="3"/>
       <c r="C16" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="17" spans="1:7" ht="17.55" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="18" spans="1:7" ht="65.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="3"/>
       <c r="B18" s="4" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="E18" t="s">
+        <v>29</v>
+      </c>
+      <c r="G18" t="s">
         <v>30</v>
-      </c>
-      <c r="G18" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="19" spans="1:7" ht="17.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="3"/>
       <c r="B19" s="3"/>
       <c r="C19" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
   </sheetData>
@@ -1332,7 +1329,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
@@ -1344,27 +1341,27 @@
   <sheetData>
     <row r="1" spans="1:5" ht="18.850000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>3</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="D1" t="s">
         <v>0</v>
       </c>
       <c r="E1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="18.850000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C2" s="2"/>
     </row>
@@ -1373,11 +1370,11 @@
         <v>4</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C3" s="1"/>
       <c r="D3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="18.850000000000001" customHeight="1" x14ac:dyDescent="0.2">
@@ -1388,18 +1385,18 @@
         <v>20130828</v>
       </c>
       <c r="D4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="41.9" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E5" t="b">
         <v>0</v>
@@ -1407,10 +1404,10 @@
     </row>
     <row r="6" spans="1:5" ht="18.850000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="B6" t="s">
         <v>156</v>
-      </c>
-      <c r="B6" t="s">
-        <v>157</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="18.850000000000001" customHeight="1" x14ac:dyDescent="0.2">
@@ -1480,8 +1477,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="12.45" x14ac:dyDescent="0.2"/>
@@ -1493,57 +1490,57 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>23</v>
-      </c>
       <c r="C1" s="2" t="s">
-        <v>6</v>
+        <v>163</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B2" t="s">
         <v>24</v>
       </c>
-      <c r="B2" t="s">
-        <v>25</v>
-      </c>
       <c r="C2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
   </sheetData>
@@ -1574,468 +1571,468 @@
   <sheetData>
     <row r="1" spans="1:3" ht="13.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1" t="s">
         <v>40</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>41</v>
-      </c>
-      <c r="C1" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="13.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B2" t="s">
         <v>43</v>
-      </c>
-      <c r="B2" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="13.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
+        <v>44</v>
+      </c>
+      <c r="B3" t="s">
         <v>45</v>
-      </c>
-      <c r="B3" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="13.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
+        <v>46</v>
+      </c>
+      <c r="B4" t="s">
         <v>47</v>
-      </c>
-      <c r="B4" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="13.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
+        <v>48</v>
+      </c>
+      <c r="B5" t="s">
         <v>49</v>
-      </c>
-      <c r="B5" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="13.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
+        <v>50</v>
+      </c>
+      <c r="B6" t="s">
         <v>51</v>
-      </c>
-      <c r="B6" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
+        <v>52</v>
+      </c>
+      <c r="B7" t="s">
         <v>53</v>
       </c>
-      <c r="B7" t="s">
+      <c r="C7" t="s">
         <v>54</v>
-      </c>
-      <c r="C7" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
+        <v>55</v>
+      </c>
+      <c r="B8" t="s">
         <v>56</v>
       </c>
-      <c r="B8" t="s">
+      <c r="C8" s="5" t="s">
         <v>57</v>
-      </c>
-      <c r="C8" s="5" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
+        <v>58</v>
+      </c>
+      <c r="B9" t="s">
         <v>59</v>
       </c>
-      <c r="B9" t="s">
+      <c r="C9" t="s">
         <v>60</v>
-      </c>
-      <c r="C9" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
+        <v>61</v>
+      </c>
+      <c r="B10" t="s">
         <v>62</v>
       </c>
-      <c r="B10" t="s">
+      <c r="C10" t="s">
         <v>63</v>
-      </c>
-      <c r="C10" t="s">
-        <v>64</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="13.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
+        <v>64</v>
+      </c>
+      <c r="B11" t="s">
         <v>65</v>
-      </c>
-      <c r="B11" t="s">
-        <v>66</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="13.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
+        <v>66</v>
+      </c>
+      <c r="B12" t="s">
         <v>67</v>
-      </c>
-      <c r="B12" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
+        <v>68</v>
+      </c>
+      <c r="B13" t="s">
         <v>69</v>
-      </c>
-      <c r="B13" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
+        <v>70</v>
+      </c>
+      <c r="B14" t="s">
         <v>71</v>
-      </c>
-      <c r="B14" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
+        <v>72</v>
+      </c>
+      <c r="B15" t="s">
         <v>73</v>
-      </c>
-      <c r="B15" t="s">
-        <v>74</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
+        <v>74</v>
+      </c>
+      <c r="B16" t="s">
         <v>75</v>
-      </c>
-      <c r="B16" t="s">
-        <v>76</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
+        <v>76</v>
+      </c>
+      <c r="B17" t="s">
         <v>77</v>
-      </c>
-      <c r="B17" t="s">
-        <v>78</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
+        <v>78</v>
+      </c>
+      <c r="B18" t="s">
         <v>79</v>
-      </c>
-      <c r="B18" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
+        <v>80</v>
+      </c>
+      <c r="B19" t="s">
         <v>81</v>
-      </c>
-      <c r="B19" t="s">
-        <v>82</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
+        <v>82</v>
+      </c>
+      <c r="B20" t="s">
         <v>83</v>
-      </c>
-      <c r="B20" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
+        <v>84</v>
+      </c>
+      <c r="B21" t="s">
         <v>85</v>
-      </c>
-      <c r="B21" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
+        <v>86</v>
+      </c>
+      <c r="B22" t="s">
         <v>87</v>
-      </c>
-      <c r="B22" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
+        <v>88</v>
+      </c>
+      <c r="B23" t="s">
         <v>89</v>
-      </c>
-      <c r="B23" t="s">
-        <v>90</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
+        <v>90</v>
+      </c>
+      <c r="B24" t="s">
         <v>91</v>
-      </c>
-      <c r="B24" t="s">
-        <v>92</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
+        <v>92</v>
+      </c>
+      <c r="B25" t="s">
         <v>93</v>
-      </c>
-      <c r="B25" t="s">
-        <v>94</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
+        <v>94</v>
+      </c>
+      <c r="B26" t="s">
         <v>95</v>
-      </c>
-      <c r="B26" t="s">
-        <v>96</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
+        <v>96</v>
+      </c>
+      <c r="B27" t="s">
         <v>97</v>
-      </c>
-      <c r="B27" t="s">
-        <v>98</v>
       </c>
     </row>
     <row r="28" spans="1:2" ht="28.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
+        <v>98</v>
+      </c>
+      <c r="B28" t="s">
         <v>99</v>
-      </c>
-      <c r="B28" t="s">
-        <v>100</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
+        <v>100</v>
+      </c>
+      <c r="B29" t="s">
         <v>101</v>
-      </c>
-      <c r="B29" t="s">
-        <v>102</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
+        <v>102</v>
+      </c>
+      <c r="B30" t="s">
         <v>103</v>
-      </c>
-      <c r="B30" t="s">
-        <v>104</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
+        <v>104</v>
+      </c>
+      <c r="B31" t="s">
         <v>105</v>
-      </c>
-      <c r="B31" t="s">
-        <v>106</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
+        <v>106</v>
+      </c>
+      <c r="B33" t="s">
         <v>107</v>
-      </c>
-      <c r="B33" t="s">
-        <v>108</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
+        <v>108</v>
+      </c>
+      <c r="B34" t="s">
         <v>109</v>
-      </c>
-      <c r="B34" t="s">
-        <v>110</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
+        <v>110</v>
+      </c>
+      <c r="B35" t="s">
         <v>111</v>
-      </c>
-      <c r="B35" t="s">
-        <v>112</v>
       </c>
     </row>
     <row r="36" spans="1:3" ht="161.69999999999999" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
+        <v>112</v>
+      </c>
+      <c r="B36" t="s">
         <v>113</v>
-      </c>
-      <c r="B36" t="s">
-        <v>114</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
+        <v>114</v>
+      </c>
+      <c r="B37" t="s">
         <v>115</v>
-      </c>
-      <c r="B37" t="s">
-        <v>116</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
+        <v>116</v>
+      </c>
+      <c r="B38" t="s">
         <v>117</v>
-      </c>
-      <c r="B38" t="s">
-        <v>118</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
+        <v>118</v>
+      </c>
+      <c r="B39" t="s">
         <v>119</v>
-      </c>
-      <c r="B39" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
+        <v>120</v>
+      </c>
+      <c r="B40" t="s">
         <v>121</v>
-      </c>
-      <c r="B40" t="s">
-        <v>122</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
+        <v>122</v>
+      </c>
+      <c r="B41" t="s">
         <v>123</v>
-      </c>
-      <c r="B41" t="s">
-        <v>124</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
+        <v>124</v>
+      </c>
+      <c r="B42" t="s">
         <v>125</v>
-      </c>
-      <c r="B42" t="s">
-        <v>126</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
+        <v>126</v>
+      </c>
+      <c r="B43" t="s">
         <v>127</v>
-      </c>
-      <c r="B43" t="s">
-        <v>128</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
+        <v>128</v>
+      </c>
+      <c r="B44" t="s">
         <v>129</v>
-      </c>
-      <c r="B44" t="s">
-        <v>130</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
+        <v>130</v>
+      </c>
+      <c r="B45" t="s">
         <v>131</v>
       </c>
-      <c r="B45" t="s">
+      <c r="C45" t="s">
         <v>132</v>
-      </c>
-      <c r="C45" t="s">
-        <v>133</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
+        <v>133</v>
+      </c>
+      <c r="B46" t="s">
         <v>134</v>
-      </c>
-      <c r="B46" t="s">
-        <v>135</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
+        <v>135</v>
+      </c>
+      <c r="B47" t="s">
         <v>136</v>
-      </c>
-      <c r="B47" t="s">
-        <v>137</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
+        <v>137</v>
+      </c>
+      <c r="B48" t="s">
         <v>138</v>
-      </c>
-      <c r="B48" t="s">
-        <v>139</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
+        <v>139</v>
+      </c>
+      <c r="B49" t="s">
         <v>140</v>
-      </c>
-      <c r="B49" t="s">
-        <v>141</v>
       </c>
     </row>
     <row r="50" spans="1:2" ht="13.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
+        <v>141</v>
+      </c>
+      <c r="B50" t="s">
         <v>142</v>
-      </c>
-      <c r="B50" t="s">
-        <v>143</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
+        <v>143</v>
+      </c>
+      <c r="B51" t="s">
         <v>144</v>
-      </c>
-      <c r="B51" t="s">
-        <v>145</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B52" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
+        <v>146</v>
+      </c>
+      <c r="B53" t="s">
         <v>147</v>
-      </c>
-      <c r="B53" t="s">
-        <v>148</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B54" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
+        <v>149</v>
+      </c>
+      <c r="B55" t="s">
         <v>150</v>
-      </c>
-      <c r="B55" t="s">
-        <v>151</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
+        <v>151</v>
+      </c>
+      <c r="B56" t="s">
         <v>152</v>
-      </c>
-      <c r="B56" t="s">
-        <v>153</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
+        <v>153</v>
+      </c>
+      <c r="B57" t="s">
         <v>154</v>
-      </c>
-      <c r="B57" t="s">
-        <v>155</v>
       </c>
     </row>
   </sheetData>

</xml_diff>